<commit_message>
WIP: Reimplement logic of pivot tables to use new data structures.
Doesn't use styles and completely buggy.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/LongText/outputfile.xlsx
+++ b/ClosedXML.Tests/Resource/Other/PivotTableReferenceFiles/LongText/outputfile.xlsx
@@ -90,34 +90,27 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable.xml><?xml version="1.0" encoding="utf-8"?>
-<x:pivotTableDefinition xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataCaption="Values" showError="0" missingCaption="" showMissing="1" pageWrap="0" pageOverThenDown="0" indent="1">
-  <x:location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <x:pivotFields count="2">
-    <x:pivotField name="Col1" axis="axisRow" showAll="0" defaultSubtotal="0">
-      <x:items count="1">
-        <x:item x="0"/>
-      </x:items>
-    </x:pivotField>
-    <x:pivotField name="Col2" defaultSubtotal="0"/>
-  </x:pivotFields>
-  <x:rowFields count="1">
-    <x:field x="0"/>
-  </x:rowFields>
-  <x:rowItems count="2">
-    <x:i>
-      <x:x v="0"/>
-    </x:i>
-    <x:i t="grand">
-      <x:x/>
-    </x:i>
-  </x:rowItems>
-  <x:pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" enableEdit="0" hideValuesRow="1"/>
-    </x:ext>
-  </x:extLst>
-</x:pivotTableDefinition>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" outline="1">
+  <location ref="A1" firstHeaderRow="0" firstDataRow="0" firstDataCol="0"/>
+  <pivotFields count="2">
+    <pivotField name="Col1" axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition enableEdit="0" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>